<commit_message>
Update the final draft after checking out
</commit_message>
<xml_diff>
--- a/Revision_Progress.xlsx
+++ b/Revision_Progress.xlsx
@@ -288,12 +288,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -308,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -316,6 +322,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,178 +733,189 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+      <c r="A21" s="3"/>
+      <c r="B21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+      <c r="A23" s="3"/>
+      <c r="B23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+      <c r="A24" s="3"/>
+      <c r="B24" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
+      <c r="A26" s="3"/>
+      <c r="B26" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
+      <c r="A27" s="3"/>
+      <c r="B27" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
+      <c r="A30" s="3"/>
+      <c r="B30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
+      <c r="A31" s="3"/>
+      <c r="B31" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="5">
         <v>0</v>
       </c>
     </row>
@@ -907,35 +931,35 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="5">
         <v>0</v>
       </c>
     </row>
@@ -972,13 +996,13 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1007,10 +1031,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="2" t="s">
+      <c r="A44" s="3"/>
+      <c r="B44" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1047,13 +1072,13 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="5">
         <v>0</v>
       </c>
     </row>

</xml_diff>